<commit_message>
Remove typo in D_Compliance_with_OECD-FATF_recommendations_on_due_diligence_OECD_2013
</commit_message>
<xml_diff>
--- a/datastatic/datasets/online/D_Compliance_with_OECD-FATF_recommendations_on_due_diligence_OECD_2013.xlsx
+++ b/datastatic/datasets/online/D_Compliance_with_OECD-FATF_recommendations_on_due_diligence_OECD_2013.xlsx
@@ -37,7 +37,7 @@
     <t>short_indicator_description$de</t>
   </si>
   <si>
-    <t>Der Indikator misst die Einhaltung der Empfehlungen der Financial Action Task Force (FATF) zur Riskioprüfung und Berichtsmaßnahmen.</t>
+    <t>Der Indikator misst die Einhaltung der Empfehlungen der Financial Action Task Force (FATF) zur Risikoprüfung und Berichtsmaßnahmen.</t>
   </si>
   <si>
     <t>short_indicator_description$en</t>
@@ -64,7 +64,7 @@
     <t>long_indicator_description$de$text</t>
   </si>
   <si>
-    <t xml:space="preserve">Menschen aus Entwicklungsländern mit illegal angeeignetem Vermögen suchen oft Wege dieses in anderen Ländern anzulegen. Sie suchen Länder mit stabilen und berechenbaren Finanzsystemen, jene Länder wo Ermittlung schwierig ist, da es nur schwache Anti-Geldwäschegesetze gibt. Untersuchungen zu den größten Korruptionsfällen der letzten Jahre zeigen, dass große Mengen an illegalen Geldsummen aus Entwicklungsländern in OECD-Länder transferiert wurden. Die FATF (Financial Action Task Force) formuliert umfassende Maßnahmen gegen Geldwäsche. Dieser Indikator misst die Einhaltung der Empfehlungen der FATF zur Riskioprüfung und Berichtsmaßnahmen (Empfehlungen 5-12). </t>
+    <t xml:space="preserve">Menschen aus Entwicklungsländern mit illegal angeeignetem Vermögen suchen oft Wege dieses in anderen Ländern anzulegen. Sie suchen Länder mit stabilen und berechenbaren Finanzsystemen, jene Länder wo Ermittlung schwierig ist, da es nur schwache Anti-Geldwäschegesetze gibt. Untersuchungen zu den größten Korruptionsfällen der letzten Jahre zeigen, dass große Mengen an illegalen Geldsummen aus Entwicklungsländern in OECD-Länder transferiert wurden. Die FATF (Financial Action Task Force) formuliert umfassende Maßnahmen gegen Geldwäsche. Dieser Indikator misst die Einhaltung der Empfehlungen der FATF zur Risikoprüfung und Berichtsmaßnahmen (Empfehlungen 5-12). </t>
   </si>
   <si>
     <t>long_indicator_description$de$baseunit</t>

</xml_diff>